<commit_message>
Add CSS and align fields properly
</commit_message>
<xml_diff>
--- a/mainapp/Employees.xlsx
+++ b/mainapp/Employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tirupati\Desktop\Presidio\EmployeeManagement\mainapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D6B210-1EBD-4804-8E18-EFDAD1837B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ACD64D-E40E-4405-9D72-008DA3DB32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -43,13 +43,10 @@
     <t>Raj sharma</t>
   </si>
   <si>
-    <t>15/10/2000</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
-    <t>Sukhi Singh</t>
+    <t>Sukhi Singh Lodhi</t>
   </si>
   <si>
     <t>HR</t>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Finance</t>
+  </si>
+  <si>
+    <t>Radhesyam kamra</t>
   </si>
 </sst>
 </file>
@@ -422,15 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -460,17 +461,17 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="C2" s="2">
+        <v>35771</v>
       </c>
       <c r="D2">
         <v>50000</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -478,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>36135</v>
@@ -487,7 +488,7 @@
         <v>48000</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>26</v>
@@ -498,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>35587</v>
@@ -507,10 +508,30 @@
         <v>56000</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>34760</v>
+      </c>
+      <c r="D5">
+        <v>47000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes and with additional employee data
</commit_message>
<xml_diff>
--- a/mainapp/Employees.xlsx
+++ b/mainapp/Employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tirupati\Desktop\Presidio\EmployeeManagement\mainapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ACD64D-E40E-4405-9D72-008DA3DB32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6F0871-305F-4666-99C9-30EAAFAEF597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,60 @@
   </si>
   <si>
     <t>Radhesyam kamra</t>
+  </si>
+  <si>
+    <t>Maya Lohar</t>
+  </si>
+  <si>
+    <t>Shyama rai</t>
+  </si>
+  <si>
+    <t>Gunjan Mehta</t>
+  </si>
+  <si>
+    <t>Vikram thakur</t>
+  </si>
+  <si>
+    <t>Abhimanyu singh</t>
+  </si>
+  <si>
+    <t>Suresh Kumar</t>
+  </si>
+  <si>
+    <t>Bharatram Patidar</t>
+  </si>
+  <si>
+    <t>Priya Sharma</t>
+  </si>
+  <si>
+    <t>Sapna Chouhan</t>
+  </si>
+  <si>
+    <t>Mohit Patidar</t>
+  </si>
+  <si>
+    <t>Kavita Laxmi</t>
+  </si>
+  <si>
+    <t>Swati Chouhan</t>
+  </si>
+  <si>
+    <t>Pradyuman Singh</t>
+  </si>
+  <si>
+    <t>Akshay Kumar</t>
+  </si>
+  <si>
+    <t>Twinkle Khanna</t>
+  </si>
+  <si>
+    <t>Sunita Patidar</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Health</t>
   </si>
 </sst>
 </file>
@@ -114,12 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,6 +589,326 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>34732</v>
+      </c>
+      <c r="D6">
+        <v>56000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>36883</v>
+      </c>
+      <c r="D7">
+        <v>23000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>34536</v>
+      </c>
+      <c r="D8">
+        <v>43000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>37061</v>
+      </c>
+      <c r="D9">
+        <v>56000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2">
+        <v>37746</v>
+      </c>
+      <c r="D10">
+        <v>12000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>37735</v>
+      </c>
+      <c r="D11">
+        <v>49000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
+        <v>35431</v>
+      </c>
+      <c r="D12">
+        <v>54000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
+        <v>36681</v>
+      </c>
+      <c r="D13">
+        <v>23000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2">
+        <v>36814</v>
+      </c>
+      <c r="D14">
+        <v>78000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2">
+        <v>35912</v>
+      </c>
+      <c r="D15">
+        <v>67000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2">
+        <v>37143</v>
+      </c>
+      <c r="D16">
+        <v>45000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2">
+        <v>38112</v>
+      </c>
+      <c r="D17">
+        <v>55000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2">
+        <v>37205</v>
+      </c>
+      <c r="D18">
+        <v>89000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2">
+        <v>37094</v>
+      </c>
+      <c r="D19">
+        <v>36000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>36496</v>
+      </c>
+      <c r="D20">
+        <v>64000</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3">
+        <v>36506</v>
+      </c>
+      <c r="D21">
+        <v>56000</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>